<commit_message>
Repetición commits por problema en el push
He tenido que anular los últimos 6 commits porque se había colapsado el "push" de GitHub Desktop al colgar imágenes muy pesadas. Entonces voy a volver a repetir esos cambios en esta tarea sin incluir dichas imágenes. A partir de ahora las imágenes irán en "gitignore".
</commit_message>
<xml_diff>
--- a/Resultados con preprocesamiento gaussiano.xlsx
+++ b/Resultados con preprocesamiento gaussiano.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\TFG\Transfer-Learning-EDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AAA0C5-4FE7-429A-BBD5-500114657E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F55DFC-E2EA-48FD-9A34-C6AC7322609C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2153,7 +2153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AE9240-3540-4FA1-BF78-BED50B4D806C}">
   <dimension ref="A2:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="129" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>